<commit_message>
トラブル一覧、start上传文件功能 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_物件管理/test_ホワイトボート_空き待ちリスト.xlsx
+++ b/test_物件管理/test_ホワイトボート_空き待ちリスト.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="822" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="822" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -4533,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:KP155"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19264,7 +19264,7 @@
   <dimension ref="B1:AH47"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -20431,8 +20431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -21958,7 +21958,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -23961,8 +23961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>